<commit_message>
Adding Financial Year Wise Data
</commit_message>
<xml_diff>
--- a/ZSS/resources/Purva Vihar/2012/06-June2012.xlsx
+++ b/ZSS/resources/Purva Vihar/2012/06-June2012.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\PurvaVihar\ACP_PV\ZSS\resources\Purva Vihar\2012\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A-June2012" sheetId="1" r:id="rId1"/>
-    <sheet name="B-June2012" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="B-June2012" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
   <si>
     <t>Name of Flat Holder</t>
   </si>
@@ -329,16 +335,127 @@
       <t>.</t>
     </r>
   </si>
+  <si>
+    <t>Map&lt;String, "String&gt; flatNameMap = new HashMap&lt;&gt;();</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("1", "Kadam R. S.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("2", "Khadtare B. B.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("7", "Devgirikar S.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("8", "Kshirsagar B. L.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("9", "Awale D.T.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("10", "Dandekar V. N.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("15", "Rathod G. H.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("16", "Arde K. Y.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("17", "Nirgude M. V.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("18", "Naidu S. M.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("23", "Dumpatti N. Y.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("24", "Remobhotkar R.B./S.B.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("25", "Ghare S. D.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("26", "Rane A. K.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("31", "Kudal P. R.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("32", "Kirve M. M.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("33", "Rajmane M. M.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("34", "Rajguru H. V.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("3", "Khadtare B. B.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("4", "Samak S. G.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("5", "Naik B. B.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("6", "Poman L. K.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("11", "Khadtare B. B.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("12", "Kulkarni S. D.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("13", "Patil K. H.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("14", "Kour R. B.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("19", "Mane M. B.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("20", "Bhise V. R.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("21", "Naik C. N.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("22", "Patil M. R.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("27", "Patil B. B.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("28A", "Phadtare Sunanda");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("28B", "Patil S. U.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("29A", "Katare");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("29B", "Ghade S. S.");</t>
+  </si>
+  <si>
+    <t>flatNameMap.put("30", "Todkar D. G.");</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,8 +486,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,8 +507,26 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -432,12 +575,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -457,8 +711,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -471,93 +729,225 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
       <font>
@@ -567,6 +957,27 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
     </dxf>
     <dxf>
       <font>
@@ -583,46 +994,60 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="AJune2012" displayName="AJune2012" ref="A9:K28" totalsRowCount="1" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="AJune2012" displayName="AJune2012" ref="A9:K28" totalsRowCount="1" headerRowDxfId="35">
   <tableColumns count="11">
-    <tableColumn id="1" name="Flat No." totalsRowLabel="Total" dataDxfId="28"/>
+    <tableColumn id="1" name="Flat No." totalsRowLabel="Total" dataDxfId="34"/>
     <tableColumn id="2" name="Name of Flat Holder" totalsRowFunction="count"/>
-    <tableColumn id="3" name="Last Month's Balance" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="5"/>
-    <tableColumn id="4" name="Current Month Balance" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="4"/>
-    <tableColumn id="5" name="Total Balance" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="3">
+    <tableColumn id="3" name="Last Month's Balance" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="11"/>
+    <tableColumn id="4" name="Current Month Balance" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="10"/>
+    <tableColumn id="5" name="Total Balance" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="9">
       <calculatedColumnFormula>AJune2012[[#This Row],[Last Month''s Balance]]+AJune2012[[#This Row],[Current Month Balance]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Penalty" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="2"/>
-    <tableColumn id="7" name="Received Maint. Charge" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="1"/>
-    <tableColumn id="11" name="Remaining Balance" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="0">
+    <tableColumn id="6" name="Penalty" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="8"/>
+    <tableColumn id="7" name="Received Maint. Charge" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="7"/>
+    <tableColumn id="11" name="Remaining Balance" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="6">
       <calculatedColumnFormula>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Date"/>
     <tableColumn id="9" name="Payer's Sign"/>
-    <tableColumn id="10" name="Receipt No." dataDxfId="14"/>
+    <tableColumn id="10" name="Receipt No." dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="BJune2012" displayName="BJune2012" ref="A9:K28" totalsRowCount="1" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C4:D40" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="C4:D40"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Flat No." dataDxfId="2"/>
+    <tableColumn id="2" name="Name of Flat Holder" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="BJune2012" displayName="BJune2012" ref="A9:K28" totalsRowCount="1" headerRowDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" name="Flat No." totalsRowLabel="Total" dataDxfId="26"/>
+    <tableColumn id="1" name="Flat No." totalsRowLabel="Total" dataDxfId="25"/>
     <tableColumn id="2" name="Name of Flat Holder" totalsRowFunction="count"/>
-    <tableColumn id="3" name="Last Month's Balance" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="11"/>
-    <tableColumn id="4" name="Current Month Balance" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="10"/>
-    <tableColumn id="5" name="Total Balance" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="9">
+    <tableColumn id="3" name="Last Month's Balance" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="4" name="Current Month Balance" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="5" name="Total Balance" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19">
       <calculatedColumnFormula>BJune2012[[#This Row],[Current Month Balance]]+BJune2012[[#This Row],[Last Month''s Balance]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Penalty" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="8"/>
-    <tableColumn id="7" name="Received Maint. Charge" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="7"/>
-    <tableColumn id="11" name="Remaining Balance" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="6">
+    <tableColumn id="6" name="Penalty" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="7" name="Received Maint. Charge" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="11" name="Remaining Balance" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13">
       <calculatedColumnFormula>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Date"/>
@@ -676,7 +1101,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -711,7 +1136,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -922,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="A9:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,30 +1367,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
@@ -978,30 +1403,30 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1065,10 +1490,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>3700</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="10">
         <v>41088</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="9">
         <v>2919</v>
       </c>
     </row>
@@ -1099,10 +1524,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>350</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="10">
         <v>41088</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="9">
         <v>2920</v>
       </c>
     </row>
@@ -1133,10 +1558,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>80</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="10">
         <v>41088</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="9">
         <v>2921</v>
       </c>
     </row>
@@ -1167,7 +1592,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>200</v>
       </c>
-      <c r="K13" s="13"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
@@ -1196,7 +1621,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>630</v>
       </c>
-      <c r="K14" s="13"/>
+      <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
@@ -1225,10 +1650,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>190</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="10">
         <v>41087</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="9">
         <v>2922</v>
       </c>
     </row>
@@ -1259,10 +1684,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>0</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="10">
         <v>41087</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="9">
         <v>2923</v>
       </c>
     </row>
@@ -1293,10 +1718,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>10</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="10">
         <v>41087</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="9">
         <v>2924</v>
       </c>
     </row>
@@ -1327,10 +1752,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>0</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="10">
         <v>41087</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="9">
         <v>2925</v>
       </c>
     </row>
@@ -1361,10 +1786,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>20</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="10">
         <v>41088</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K19" s="9">
         <v>2926</v>
       </c>
     </row>
@@ -1395,10 +1820,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>10</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="10">
         <v>41087</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="9">
         <v>2927</v>
       </c>
     </row>
@@ -1429,10 +1854,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>-200</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="10">
         <v>41087</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="9">
         <v>2928</v>
       </c>
     </row>
@@ -1463,10 +1888,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>0</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="10">
         <v>41087</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="9">
         <v>2929</v>
       </c>
     </row>
@@ -1497,10 +1922,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>30</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="10">
         <v>41070</v>
       </c>
-      <c r="K23" s="13">
+      <c r="K23" s="9">
         <v>2930</v>
       </c>
     </row>
@@ -1531,10 +1956,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>7360</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="10">
         <v>41087</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="9">
         <v>2931</v>
       </c>
     </row>
@@ -1565,7 +1990,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>-300</v>
       </c>
-      <c r="K25" s="13"/>
+      <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -1594,7 +2019,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>3600</v>
       </c>
-      <c r="K26" s="13"/>
+      <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -1623,7 +2048,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>1480</v>
       </c>
-      <c r="K27" s="13"/>
+      <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1659,32 +2084,32 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1704,10 +2129,440 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:H40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="17">
+        <v>2</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="16">
+        <v>7</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="17">
+        <v>8</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="16">
+        <v>9</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="17">
+        <v>10</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="16">
+        <v>15</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="17">
+        <v>16</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="16">
+        <v>17</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="17">
+        <v>18</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="16">
+        <v>23</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="17">
+        <v>24</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="16">
+        <v>25</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="17">
+        <v>26</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="16">
+        <v>31</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="17">
+        <v>32</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="16">
+        <v>33</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="17">
+        <v>34</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="16">
+        <v>3</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="17">
+        <v>4</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="16">
+        <v>5</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="17">
+        <v>6</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="16">
+        <v>11</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="17">
+        <v>12</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="16">
+        <v>13</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="17">
+        <v>14</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="16">
+        <v>19</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="17">
+        <v>20</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="16">
+        <v>21</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="17">
+        <v>22</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="16">
+        <v>27</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="21">
+        <v>30</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H40" s="26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K31"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H27" sqref="H10:H27"/>
+      <selection activeCell="A10" sqref="A10:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,30 +2580,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
@@ -1761,30 +2616,30 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1848,10 +2703,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>290</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="10">
         <v>41086</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="9">
         <v>2932</v>
       </c>
     </row>
@@ -1882,7 +2737,7 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>930</v>
       </c>
-      <c r="K11" s="13"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
@@ -1911,10 +2766,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>40</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="10">
         <v>41086</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="9">
         <v>2933</v>
       </c>
     </row>
@@ -1945,10 +2800,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="10">
         <v>41088</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="9">
         <v>2934</v>
       </c>
     </row>
@@ -1979,10 +2834,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="10">
         <v>41086</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="9">
         <v>2935</v>
       </c>
     </row>
@@ -2013,10 +2868,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>2130</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="10">
         <v>41086</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="9">
         <v>2936</v>
       </c>
     </row>
@@ -2047,7 +2902,7 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>2480</v>
       </c>
-      <c r="K16" s="13"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
@@ -2076,10 +2931,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="10">
         <v>41086</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="9">
         <v>2937</v>
       </c>
     </row>
@@ -2110,10 +2965,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>30</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="10">
         <v>41088</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="9">
         <v>2938</v>
       </c>
     </row>
@@ -2144,10 +2999,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>80</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="10">
         <v>41070</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K19" s="9">
         <v>2939</v>
       </c>
     </row>
@@ -2178,10 +3033,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>40</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="10">
         <v>41086</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="9">
         <v>2940</v>
       </c>
     </row>
@@ -2212,10 +3067,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="10">
         <v>41086</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="9">
         <v>2941</v>
       </c>
     </row>
@@ -2246,10 +3101,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="10">
         <v>41086</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="9">
         <v>2942</v>
       </c>
     </row>
@@ -2280,10 +3135,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>2850</v>
       </c>
-      <c r="I23" s="14">
+      <c r="I23" s="10">
         <v>41070</v>
       </c>
-      <c r="K23" s="13">
+      <c r="K23" s="9">
         <v>2943</v>
       </c>
     </row>
@@ -2314,10 +3169,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="10">
         <v>41086</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="9">
         <v>2944</v>
       </c>
     </row>
@@ -2348,10 +3203,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>330</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I25" s="10">
         <v>41088</v>
       </c>
-      <c r="K25" s="13">
+      <c r="K25" s="9">
         <v>2945</v>
       </c>
     </row>
@@ -2382,10 +3237,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="10">
         <v>41086</v>
       </c>
-      <c r="K26" s="13">
+      <c r="K26" s="9">
         <v>2946</v>
       </c>
     </row>
@@ -2416,10 +3271,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="10">
         <v>41086</v>
       </c>
-      <c r="K27" s="13">
+      <c r="K27" s="9">
         <v>2947</v>
       </c>
     </row>
@@ -2457,32 +3312,32 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Revert "Adding Financial Year Wise Data"
</commit_message>
<xml_diff>
--- a/ZSS/resources/Purva Vihar/2012/06-June2012.xlsx
+++ b/ZSS/resources/Purva Vihar/2012/06-June2012.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\PurvaVihar\ACP_PV\ZSS\resources\Purva Vihar\2012\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="A-June2012" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="B-June2012" sheetId="3" r:id="rId3"/>
+    <sheet name="B-June2012" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Name of Flat Holder</t>
   </si>
@@ -335,127 +329,16 @@
       <t>.</t>
     </r>
   </si>
-  <si>
-    <t>Map&lt;String, "String&gt; flatNameMap = new HashMap&lt;&gt;();</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("1", "Kadam R. S.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("2", "Khadtare B. B.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("7", "Devgirikar S.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("8", "Kshirsagar B. L.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("9", "Awale D.T.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("10", "Dandekar V. N.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("15", "Rathod G. H.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("16", "Arde K. Y.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("17", "Nirgude M. V.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("18", "Naidu S. M.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("23", "Dumpatti N. Y.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("24", "Remobhotkar R.B./S.B.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("25", "Ghare S. D.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("26", "Rane A. K.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("31", "Kudal P. R.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("32", "Kirve M. M.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("33", "Rajmane M. M.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("34", "Rajguru H. V.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("3", "Khadtare B. B.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("4", "Samak S. G.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("5", "Naik B. B.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("6", "Poman L. K.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("11", "Khadtare B. B.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("12", "Kulkarni S. D.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("13", "Patil K. H.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("14", "Kour R. B.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("19", "Mane M. B.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("20", "Bhise V. R.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("21", "Naik C. N.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("22", "Patil M. R.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("27", "Patil B. B.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("28A", "Phadtare Sunanda");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("28B", "Patil S. U.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("29A", "Katare");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("29B", "Ghade S. S.");</t>
-  </si>
-  <si>
-    <t>flatNameMap.put("30", "Todkar D. G.");</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -486,16 +369,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,26 +382,8 @@
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor theme="4" tint="0.59999389629810485"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -575,123 +432,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -711,12 +457,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -729,225 +471,93 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+  <dxfs count="30">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
       <font>
@@ -957,27 +567,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_ [$रु-44E]\ * #,##0_ ;_ [$रु-44E]\ * \-#,##0_ ;_ [$रु-44E]\ * &quot;-&quot;_ ;_ @_ "/>
     </dxf>
     <dxf>
       <font>
@@ -994,60 +583,46 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="AJune2012" displayName="AJune2012" ref="A9:K28" totalsRowCount="1" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="AJune2012" displayName="AJune2012" ref="A9:K28" totalsRowCount="1" headerRowDxfId="29">
   <tableColumns count="11">
-    <tableColumn id="1" name="Flat No." totalsRowLabel="Total" dataDxfId="34"/>
+    <tableColumn id="1" name="Flat No." totalsRowLabel="Total" dataDxfId="28"/>
     <tableColumn id="2" name="Name of Flat Holder" totalsRowFunction="count"/>
-    <tableColumn id="3" name="Last Month's Balance" totalsRowFunction="sum" dataDxfId="33" totalsRowDxfId="11"/>
-    <tableColumn id="4" name="Current Month Balance" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="10"/>
-    <tableColumn id="5" name="Total Balance" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="9">
+    <tableColumn id="3" name="Last Month's Balance" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="5"/>
+    <tableColumn id="4" name="Current Month Balance" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="4"/>
+    <tableColumn id="5" name="Total Balance" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="3">
       <calculatedColumnFormula>AJune2012[[#This Row],[Last Month''s Balance]]+AJune2012[[#This Row],[Current Month Balance]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Penalty" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="8"/>
-    <tableColumn id="7" name="Received Maint. Charge" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="7"/>
-    <tableColumn id="11" name="Remaining Balance" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="6">
+    <tableColumn id="6" name="Penalty" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="2"/>
+    <tableColumn id="7" name="Received Maint. Charge" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="1"/>
+    <tableColumn id="11" name="Remaining Balance" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="0">
       <calculatedColumnFormula>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Date"/>
     <tableColumn id="9" name="Payer's Sign"/>
-    <tableColumn id="10" name="Receipt No." dataDxfId="27"/>
+    <tableColumn id="10" name="Receipt No." dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C4:D40" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
-  <autoFilter ref="C4:D40"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Flat No." dataDxfId="2"/>
-    <tableColumn id="2" name="Name of Flat Holder" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="BJune2012" displayName="BJune2012" ref="A9:K28" totalsRowCount="1" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="BJune2012" displayName="BJune2012" ref="A9:K28" totalsRowCount="1" headerRowDxfId="27">
   <tableColumns count="11">
-    <tableColumn id="1" name="Flat No." totalsRowLabel="Total" dataDxfId="25"/>
+    <tableColumn id="1" name="Flat No." totalsRowLabel="Total" dataDxfId="26"/>
     <tableColumn id="2" name="Name of Flat Holder" totalsRowFunction="count"/>
-    <tableColumn id="3" name="Last Month's Balance" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="4" name="Current Month Balance" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="5" name="Total Balance" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19">
+    <tableColumn id="3" name="Last Month's Balance" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="11"/>
+    <tableColumn id="4" name="Current Month Balance" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="10"/>
+    <tableColumn id="5" name="Total Balance" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="9">
       <calculatedColumnFormula>BJune2012[[#This Row],[Current Month Balance]]+BJune2012[[#This Row],[Last Month''s Balance]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Penalty" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="7" name="Received Maint. Charge" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="11" name="Remaining Balance" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13">
+    <tableColumn id="6" name="Penalty" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="8"/>
+    <tableColumn id="7" name="Received Maint. Charge" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="7"/>
+    <tableColumn id="11" name="Remaining Balance" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="6">
       <calculatedColumnFormula>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Date"/>
@@ -1101,7 +676,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1136,7 +711,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1347,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="A9:B27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,30 +942,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
@@ -1403,30 +978,30 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1490,10 +1065,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>3700</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="14">
         <v>41088</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="13">
         <v>2919</v>
       </c>
     </row>
@@ -1524,10 +1099,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>350</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="14">
         <v>41088</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="13">
         <v>2920</v>
       </c>
     </row>
@@ -1558,10 +1133,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>80</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="14">
         <v>41088</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="13">
         <v>2921</v>
       </c>
     </row>
@@ -1592,7 +1167,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>200</v>
       </c>
-      <c r="K13" s="9"/>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
@@ -1621,7 +1196,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>630</v>
       </c>
-      <c r="K14" s="9"/>
+      <c r="K14" s="13"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
@@ -1650,10 +1225,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>190</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="14">
         <v>41087</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="13">
         <v>2922</v>
       </c>
     </row>
@@ -1684,10 +1259,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>0</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="14">
         <v>41087</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="13">
         <v>2923</v>
       </c>
     </row>
@@ -1718,10 +1293,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>10</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="14">
         <v>41087</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="13">
         <v>2924</v>
       </c>
     </row>
@@ -1752,10 +1327,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>0</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="14">
         <v>41087</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="13">
         <v>2925</v>
       </c>
     </row>
@@ -1786,10 +1361,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>20</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="14">
         <v>41088</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="13">
         <v>2926</v>
       </c>
     </row>
@@ -1820,10 +1395,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>10</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="14">
         <v>41087</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="13">
         <v>2927</v>
       </c>
     </row>
@@ -1854,10 +1429,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>-200</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="14">
         <v>41087</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="13">
         <v>2928</v>
       </c>
     </row>
@@ -1888,10 +1463,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>0</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="14">
         <v>41087</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="13">
         <v>2929</v>
       </c>
     </row>
@@ -1922,10 +1497,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>30</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="14">
         <v>41070</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="13">
         <v>2930</v>
       </c>
     </row>
@@ -1956,10 +1531,10 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>7360</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="14">
         <v>41087</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="13">
         <v>2931</v>
       </c>
     </row>
@@ -1990,7 +1565,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>-300</v>
       </c>
-      <c r="K25" s="9"/>
+      <c r="K25" s="13"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -2019,7 +1594,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>3600</v>
       </c>
-      <c r="K26" s="9"/>
+      <c r="K26" s="13"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -2048,7 +1623,7 @@
         <f>AJune2012[[#This Row],[Total Balance]]-AJune2012[[#This Row],[Received Maint. Charge]]+AJune2012[[#This Row],[Penalty]]</f>
         <v>1480</v>
       </c>
-      <c r="K27" s="9"/>
+      <c r="K27" s="13"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2084,32 +1659,32 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2129,440 +1704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:H40"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="3:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="16">
-        <v>1</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="17">
-        <v>2</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="16">
-        <v>7</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="17">
-        <v>8</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="16">
-        <v>9</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="17">
-        <v>10</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="16">
-        <v>15</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="17">
-        <v>16</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="16">
-        <v>17</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="17">
-        <v>18</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="16">
-        <v>23</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="17">
-        <v>24</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="16">
-        <v>25</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="17">
-        <v>26</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="16">
-        <v>31</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="17">
-        <v>32</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="16">
-        <v>33</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="17">
-        <v>34</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="16">
-        <v>3</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="17">
-        <v>4</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="16">
-        <v>5</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="17">
-        <v>6</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="H26" s="25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="16">
-        <v>11</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="17">
-        <v>12</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H28" s="25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="16">
-        <v>13</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="17">
-        <v>14</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H30" s="25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="16">
-        <v>19</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H31" s="24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="17">
-        <v>20</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="H32" s="25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="16">
-        <v>21</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="H33" s="24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="17">
-        <v>22</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="H34" s="25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="16">
-        <v>27</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" s="25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="H37" s="24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H39" s="24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C40" s="21">
-        <v>30</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H40" s="26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K31"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B27"/>
+      <selection activeCell="H27" sqref="H10:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2580,30 +1725,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
@@ -2616,30 +1761,30 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -2703,10 +1848,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>290</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="14">
         <v>41086</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="13">
         <v>2932</v>
       </c>
     </row>
@@ -2737,7 +1882,7 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>930</v>
       </c>
-      <c r="K11" s="9"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
@@ -2766,10 +1911,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>40</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="14">
         <v>41086</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="13">
         <v>2933</v>
       </c>
     </row>
@@ -2800,10 +1945,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="14">
         <v>41088</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="13">
         <v>2934</v>
       </c>
     </row>
@@ -2834,10 +1979,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="14">
         <v>41086</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="13">
         <v>2935</v>
       </c>
     </row>
@@ -2868,10 +2013,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>2130</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="14">
         <v>41086</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="13">
         <v>2936</v>
       </c>
     </row>
@@ -2902,7 +2047,7 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>2480</v>
       </c>
-      <c r="K16" s="9"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
@@ -2931,10 +2076,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="14">
         <v>41086</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="13">
         <v>2937</v>
       </c>
     </row>
@@ -2965,10 +2110,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>30</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="14">
         <v>41088</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="13">
         <v>2938</v>
       </c>
     </row>
@@ -2999,10 +2144,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>80</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="14">
         <v>41070</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="13">
         <v>2939</v>
       </c>
     </row>
@@ -3033,10 +2178,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>40</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="14">
         <v>41086</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="13">
         <v>2940</v>
       </c>
     </row>
@@ -3067,10 +2212,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="14">
         <v>41086</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="13">
         <v>2941</v>
       </c>
     </row>
@@ -3101,10 +2246,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="14">
         <v>41086</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="13">
         <v>2942</v>
       </c>
     </row>
@@ -3135,10 +2280,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>2850</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="14">
         <v>41070</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="13">
         <v>2943</v>
       </c>
     </row>
@@ -3169,10 +2314,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="14">
         <v>41086</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="13">
         <v>2944</v>
       </c>
     </row>
@@ -3203,10 +2348,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>330</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="14">
         <v>41088</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="13">
         <v>2945</v>
       </c>
     </row>
@@ -3237,10 +2382,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="14">
         <v>41086</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="13">
         <v>2946</v>
       </c>
     </row>
@@ -3271,10 +2416,10 @@
         <f>BJune2012[[#This Row],[Total Balance]]+BJune2012[[#This Row],[Penalty]]-BJune2012[[#This Row],[Received Maint. Charge]]</f>
         <v>0</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="14">
         <v>41086</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="13">
         <v>2947</v>
       </c>
     </row>
@@ -3312,32 +2457,32 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>